<commit_message>
DataProvider iteration , one data provider for all test cases
</commit_message>
<xml_diff>
--- a/INB_Auotomation/src/test/resources/excel/testData.xlsx
+++ b/INB_Auotomation/src/test/resources/excel/testData.xlsx
@@ -8,15 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
   <si>
     <t>testname</t>
   </si>
@@ -48,23 +47,51 @@
     <t>2</t>
   </si>
   <si>
+    <t>To check whether the user can successfully login and logout</t>
+  </si>
+  <si>
     <t>yes</t>
   </si>
   <si>
-    <t>To check whether the user can successfully login and logout</t>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>CIF1</t>
+  </si>
+  <si>
+    <t>Asdf@123</t>
+  </si>
+  <si>
+    <t>CIF4</t>
+  </si>
+  <si>
+    <t>Asdf@333</t>
+  </si>
+  <si>
+    <t>Asdfg@123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,14 +111,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -387,7 +420,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -418,10 +451,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -438,7 +471,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
@@ -457,24 +490,112 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
multi browser testing code updated
</commit_message>
<xml_diff>
--- a/INB_Auotomation/src/test/resources/excel/testData.xlsx
+++ b/INB_Auotomation/src/test/resources/excel/testData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>testname</t>
   </si>
@@ -78,6 +78,21 @@
   </si>
   <si>
     <t>CIF2</t>
+  </si>
+  <si>
+    <t>Asdf@1234</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>microedge</t>
   </si>
 </sst>
 </file>
@@ -496,21 +511,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="2" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -518,13 +533,16 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -532,13 +550,16 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -546,13 +567,16 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -560,13 +584,16 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -574,13 +601,16 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -588,19 +618,22 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Custom Annotations Implementation in framework- kiran jadhav-18/10/22
</commit_message>
<xml_diff>
--- a/INB_Auotomation/src/test/resources/excel/testData.xlsx
+++ b/INB_Auotomation/src/test/resources/excel/testData.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
-    <sheet name="DATA" sheetId="2" r:id="rId2"/>
+    <sheet name="RETAIL_DATA" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>testname</t>
   </si>
@@ -35,64 +35,40 @@
     <t>LoginLogoutTest</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>To check whether the user can successfully login and logout</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>spcbtest</t>
+  </si>
+  <si>
+    <t>Asdf@123</t>
+  </si>
+  <si>
     <t>newTest</t>
   </si>
   <si>
-    <t>To check this testcase executed</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>To check whether the user can successfully login and logout</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>CIF1</t>
-  </si>
-  <si>
-    <t>Asdf@123</t>
-  </si>
-  <si>
-    <t>CIF4</t>
-  </si>
-  <si>
-    <t>Asdf@333</t>
-  </si>
-  <si>
-    <t>Asdfg@123</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>CIF2</t>
-  </si>
-  <si>
-    <t>Asdf@1234</t>
-  </si>
-  <si>
-    <t>browser</t>
+    <t>To check this test runs</t>
+  </si>
+  <si>
+    <t>spcb</t>
   </si>
   <si>
     <t>chrome</t>
-  </si>
-  <si>
-    <t>firefox</t>
-  </si>
-  <si>
-    <t>microedge</t>
   </si>
 </sst>
 </file>
@@ -440,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -472,49 +448,49 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="E2 E3 D2:D3" numberStoredAsText="1"/>
+    <ignoredError sqref="E2 D2 D3:E3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -533,13 +509,13 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -547,93 +523,51 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="E7" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
little changes done in framework constants files 18-10
</commit_message>
<xml_diff>
--- a/INB_Auotomation/src/test/resources/excel/testData.xlsx
+++ b/INB_Auotomation/src/test/resources/excel/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -15,22 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
-  <si>
-    <t>testname</t>
-  </si>
-  <si>
-    <t>testDescription</t>
-  </si>
-  <si>
-    <t>execute</t>
-  </si>
-  <si>
-    <t>priority</t>
-  </si>
-  <si>
-    <t>count</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>LoginLogoutTest</t>
   </si>
@@ -44,15 +29,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>browser</t>
-  </si>
-  <si>
     <t>spcbtest</t>
   </si>
   <si>
@@ -69,6 +45,42 @@
   </si>
   <si>
     <t>chrome</t>
+  </si>
+  <si>
+    <t>data1</t>
+  </si>
+  <si>
+    <t>data2</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Test Case Name</t>
+  </si>
+  <si>
+    <t>Execute</t>
+  </si>
+  <si>
+    <t>Test Description</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Login Password</t>
+  </si>
+  <si>
+    <t>User name</t>
   </si>
 </sst>
 </file>
@@ -416,8 +428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -428,53 +440,53 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -487,10 +499,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -499,75 +511,81 @@
     <col min="2" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="E7" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Test case updated 20-10
</commit_message>
<xml_diff>
--- a/INB_Auotomation/src/test/resources/excel/testData.xlsx
+++ b/INB_Auotomation/src/test/resources/excel/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -15,17 +15,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
-  <si>
-    <t>LoginLogoutTest</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>To check whether the user can successfully login and logout</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -35,52 +29,70 @@
     <t>Asdf@123</t>
   </si>
   <si>
-    <t>newTest</t>
-  </si>
-  <si>
-    <t>To check this test runs</t>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>data1</t>
+  </si>
+  <si>
+    <t>data2</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Test Case Name</t>
+  </si>
+  <si>
+    <t>Execute</t>
+  </si>
+  <si>
+    <t>Test Description</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>Login Password</t>
+  </si>
+  <si>
+    <t>User name</t>
+  </si>
+  <si>
+    <t>To Login into the application</t>
+  </si>
+  <si>
+    <t>RetailLoginLogout</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>myAccountsSummary</t>
+  </si>
+  <si>
+    <t>myAccountsStatement</t>
+  </si>
+  <si>
+    <t>To check Mouse Hover functionality on My Account menu</t>
+  </si>
+  <si>
+    <t>To check account statement</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
   <si>
     <t>spcb</t>
-  </si>
-  <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>data1</t>
-  </si>
-  <si>
-    <t>data2</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Test Case Name</t>
-  </si>
-  <si>
-    <t>Execute</t>
-  </si>
-  <si>
-    <t>Test Description</t>
-  </si>
-  <si>
-    <t>Priority</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
-    <t>Browser</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>Login Password</t>
-  </si>
-  <si>
-    <t>User name</t>
   </si>
 </sst>
 </file>
@@ -426,88 +438,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
     <col min="2" max="2" width="54.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="D5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="E2 D2 D3:E3" numberStoredAsText="1"/>
+    <ignoredError sqref="D2:E2 E3 D3:D4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="17.140625" customWidth="1"/>
@@ -516,76 +550,94 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>5</v>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1"/>
     <hyperlink ref="E4" r:id="rId2"/>
+    <hyperlink ref="E5" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
addition of test cases
</commit_message>
<xml_diff>
--- a/INB_Auotomation/src/test/resources/excel/testData.xlsx
+++ b/INB_Auotomation/src/test/resources/excel/testData.xlsx
@@ -11,12 +11,11 @@
     <sheet name="RETAIL_DATA" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A4:F19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="41">
   <si>
     <t>yes</t>
   </si>
@@ -45,9 +44,6 @@
     <t>Test Description</t>
   </si>
   <si>
-    <t>Priority</t>
-  </si>
-  <si>
     <t>Count</t>
   </si>
   <si>
@@ -75,12 +71,6 @@
     <t>to check this tests runs</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -102,9 +92,6 @@
     <t>myAccountsClick</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>requestMH</t>
   </si>
   <si>
@@ -135,7 +122,22 @@
     <t>checking Enquiry menu with click  method</t>
   </si>
   <si>
+    <t>quickLinksCheck</t>
+  </si>
+  <si>
+    <t>checking dashboard quick linnks</t>
+  </si>
+  <si>
+    <t>spcb</t>
+  </si>
+  <si>
     <t>spcbtest</t>
+  </si>
+  <si>
+    <t>profileLinksMH</t>
+  </si>
+  <si>
+    <t>checking profileLinks</t>
   </si>
 </sst>
 </file>
@@ -481,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -493,7 +495,7 @@
     <col min="2" max="2" width="54.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -506,194 +508,189 @@
       <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
         <v>26</v>
       </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>15</v>
+      <c r="D13" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D2:F3 F7 F6 E6 E7 E5:F5 E4:F4" numberStoredAsText="1"/>
+    <ignoredError sqref="D2:E3 E7 E6 D6 D7 D5:E5 D4:E4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -713,7 +710,7 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -733,24 +730,24 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
@@ -758,16 +755,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>1</v>
@@ -775,16 +772,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>1</v>
@@ -792,16 +789,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>1</v>
@@ -809,16 +806,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>1</v>
@@ -826,16 +823,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>1</v>
@@ -843,16 +840,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>1</v>
@@ -860,16 +857,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>1</v>
@@ -877,16 +874,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>1</v>
@@ -894,18 +891,52 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
         <v>0</v>
       </c>
-      <c r="C12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -921,6 +952,8 @@
     <hyperlink ref="E10" r:id="rId8"/>
     <hyperlink ref="E11" r:id="rId9"/>
     <hyperlink ref="E12" r:id="rId10"/>
+    <hyperlink ref="E13" r:id="rId11"/>
+    <hyperlink ref="E14" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>